<commit_message>
Try swimming with new adv-diff
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_Matlab.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_Matlab.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="73">
   <si>
     <t xml:space="preserve">Percent change in mass from start in percent (neg=loss) </t>
   </si>
@@ -227,7 +227,28 @@
     <t>Swim-Advect-Diffuse</t>
   </si>
   <si>
+    <t>velocity, daily 2000, bio=100, dt=1 hr, shallow</t>
+  </si>
+  <si>
     <t>velocity, daily 2000, bio=100, dt=1 hr, deep</t>
+  </si>
+  <si>
+    <t>velocity, daily 2000, bio=100, dt=1 hr, temp const</t>
+  </si>
+  <si>
+    <t>velocity, daily 2000, bio=100, dt=1 hr, temp daily</t>
+  </si>
+  <si>
+    <t>velocity, daily 2000, bio=100, dt=1 hr, zoop const</t>
+  </si>
+  <si>
+    <t>velocity, daily 2000, bio=100, dt=1 hr, zoop daily</t>
+  </si>
+  <si>
+    <t>Swim-Advect</t>
+  </si>
+  <si>
+    <t>Swim</t>
   </si>
 </sst>
 </file>
@@ -1031,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1665,10 +1686,252 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6">
+        <v>0.1191</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>65</v>
       </c>
-      <c r="F65" s="6">
-        <v>5.5221999999999997E-4</v>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6">
+        <v>-0.17849999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6">
+        <v>12.385999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6">
+        <v>0.81820000000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6">
+        <v>0.2999</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6">
+        <v>0.3306</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" s="6"/>
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6">
+        <v>0.68069999999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>65</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6">
+        <v>-1.3599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6">
+        <v>90.748699999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6">
+        <v>3.2086000000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6">
+        <v>0.98870000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6">
+        <v>0.63880000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" s="6"/>
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>66</v>
+      </c>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6">
+        <v>75.870999999999995</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>65</v>
+      </c>
+      <c r="B82" s="6"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" s="6"/>
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6">
+        <v>276.39269999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>68</v>
+      </c>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6">
+        <v>3.2787999999999999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6">
+        <v>276.52589999999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>70</v>
+      </c>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6">
+        <v>132.62020000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try swimming using nu grad
Try diffusion method of using gradient to move fish instead of
adjusting vel to cell with max.
Doesn’t move fish enough.
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_Matlab.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_Matlab.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
   <si>
     <t xml:space="preserve">Percent change in mass from start in percent (neg=loss) </t>
   </si>
@@ -249,6 +249,48 @@
   </si>
   <si>
     <t>Swim</t>
+  </si>
+  <si>
+    <t>max, daily 2000, bio=100, dt=1 hr, deep</t>
+  </si>
+  <si>
+    <t>max, daily 2000, bio=100, dt=1 hr, shallow</t>
+  </si>
+  <si>
+    <t>max, daily 2000, bio=100, dt=1 hr, temp const</t>
+  </si>
+  <si>
+    <t>max, daily 2000, bio=100, dt=1 hr, temp daily</t>
+  </si>
+  <si>
+    <t>max, daily 2000, bio=100, dt=1 hr, zoop const</t>
+  </si>
+  <si>
+    <t>max, daily 2000, bio=100, dt=1 hr, zoop daily</t>
+  </si>
+  <si>
+    <t>grad, daily 2000, bio=100, dt=1 hr, deep</t>
+  </si>
+  <si>
+    <t>grad, daily 2000, bio=100, dt=1 hr, temp const</t>
+  </si>
+  <si>
+    <t>grad, daily 2000, bio=100, dt=1 hr, shallow</t>
+  </si>
+  <si>
+    <t>grad, daily 2000, bio=100, dt=1 hr, temp daily</t>
+  </si>
+  <si>
+    <t>grad, daily 2000, bio=100, dt=1 hr, zoop const</t>
+  </si>
+  <si>
+    <t>grad, daily 2000, bio=100, dt=1 hr,zoop daily</t>
+  </si>
+  <si>
+    <t>Not enough change in distribution</t>
+  </si>
+  <si>
+    <t>Unstable</t>
   </si>
 </sst>
 </file>
@@ -1052,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1862,9 +1904,9 @@
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -1874,9 +1916,9 @@
         <v>75.870999999999995</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -1886,21 +1928,24 @@
         <v>1.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>67</v>
-      </c>
-      <c r="B83" s="6"/>
+        <v>75</v>
+      </c>
+      <c r="B83" s="6">
+        <v>-4.4668999999999999E-13</v>
+      </c>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6">
         <v>276.39269999999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83" s="6"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -1910,9 +1955,9 @@
         <v>3.2787999999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -1922,9 +1967,9 @@
         <v>276.52589999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -1932,6 +1977,48 @@
       <c r="E86" s="6"/>
       <c r="F86" s="6">
         <v>132.62020000000001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>79</v>
+      </c>
+      <c r="F87">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="G87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>80</v>
+      </c>
+      <c r="F89" s="6">
+        <v>-2.1473E-4</v>
+      </c>
+      <c r="G89" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Advection stand alone routine
</commit_message>
<xml_diff>
--- a/CODE/Data/CSV/mass_conserv_advect_Matlab.xlsx
+++ b/CODE/Data/CSV/mass_conserv_advect_Matlab.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15400" yWindow="460" windowWidth="22960" windowHeight="16520" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="20780" yWindow="460" windowWidth="17620" windowHeight="17040" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="adv" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="91">
   <si>
     <t xml:space="preserve">Percent change in mass from start in percent (neg=loss) </t>
   </si>
@@ -291,6 +291,18 @@
   </si>
   <si>
     <t>Unstable</t>
+  </si>
+  <si>
+    <t>old code, velocity, daily Core 2000, bio=100, dt=1 hr</t>
+  </si>
+  <si>
+    <t>old code, velocity, daily Core 1988, bio=100, dt=1 hr</t>
+  </si>
+  <si>
+    <t>Grad incr Eq</t>
+  </si>
+  <si>
+    <t>Grad incr Poles</t>
   </si>
 </sst>
 </file>
@@ -341,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -371,6 +383,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -700,17 +715,17 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
       <c r="L3" s="3" t="s">
         <v>2</v>
       </c>
@@ -848,17 +863,17 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
       <c r="L3" s="3" t="s">
         <v>2</v>
       </c>
@@ -977,17 +992,17 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
       <c r="L3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1094,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,7 +1120,7 @@
     <col min="1" max="1" width="41.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1129,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -1123,16 +1138,18 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1151,11 +1168,17 @@
       <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1164,13 +1187,15 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1185,11 +1210,13 @@
       <c r="F7" s="6">
         <v>6.2463000000000004E-4</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1200,16 +1227,18 @@
       <c r="F8" s="6">
         <v>6.6525000000000004E-4</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1224,11 +1253,13 @@
       <c r="F11" s="6">
         <v>5.7653000000000001E-4</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -1239,16 +1270,18 @@
       <c r="F12" s="6">
         <v>2.6260999999999998E-4</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1263,11 +1296,13 @@
       <c r="F15" s="10">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1284,11 +1319,13 @@
       <c r="F16" s="6">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1299,11 +1336,13 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" t="s">
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -1314,16 +1353,18 @@
       <c r="F18" s="6">
         <v>2.812E-4</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1334,16 +1375,18 @@
       <c r="F21" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1358,16 +1401,18 @@
       <c r="F24" s="6">
         <v>3.2924000000000001E-4</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1382,8 +1427,10 @@
       <c r="F27" s="6">
         <v>7.5767E-4</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1394,8 +1441,10 @@
       <c r="F28" s="6">
         <v>7.8421999999999997E-4</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1406,16 +1455,18 @@
       <c r="F29" s="6">
         <v>5.3474999999999996E-4</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1430,11 +1481,13 @@
       <c r="F32" s="6">
         <v>7.7035999999999999E-4</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1449,8 +1502,10 @@
       <c r="F33" s="6">
         <v>7.7523000000000002E-4</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -1465,8 +1520,10 @@
       <c r="F34" s="6">
         <v>7.7523000000000002E-4</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1481,8 +1538,10 @@
       <c r="F35" s="6">
         <v>7.7523000000000002E-4</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -1493,16 +1552,18 @@
       <c r="F36" s="6">
         <v>5.5221999999999997E-4</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1513,16 +1574,18 @@
       <c r="F39" s="6">
         <v>3.6789E-4</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -1532,8 +1595,10 @@
       <c r="F43" s="6">
         <v>-1.6154999999999999E-12</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -1543,8 +1608,10 @@
       <c r="F44" s="6">
         <v>-1.4261E-12</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -1554,11 +1621,13 @@
       <c r="F45" s="6">
         <v>-1.6154999999999999E-12</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -1571,11 +1640,11 @@
       <c r="E46" s="6">
         <v>-3.4775000000000002E-6</v>
       </c>
-      <c r="G46" t="s">
+      <c r="I46" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1588,8 +1657,10 @@
       <c r="F47" s="6">
         <v>-2.6516000000000001E-12</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -1602,10 +1673,12 @@
       <c r="F48" s="6">
         <v>-2.0053999999999999E-12</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="B49" s="6">
         <v>4.7473999999999995E-13</v>
@@ -1616,21 +1689,26 @@
       <c r="F49" s="6">
         <v>-1.2924E-12</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6">
+        <v>-3.3423999999999997E-14</v>
+      </c>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>53</v>
-      </c>
-      <c r="B50" s="6">
-        <v>2.1793999999999998E-5</v>
-      </c>
-      <c r="F50" s="12">
-        <v>1.3675999999999999E-5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>54</v>
       </c>
       <c r="B51" s="6">
         <v>2.1793999999999998E-5</v>
@@ -1638,386 +1716,482 @@
       <c r="F51" s="12">
         <v>1.3675999999999999E-5</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" s="6">
         <v>2.1793999999999998E-5</v>
       </c>
-      <c r="F52" s="12"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F52" s="12">
+        <v>1.3675999999999999E-5</v>
+      </c>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="6">
+        <v>2.1793999999999998E-5</v>
+      </c>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>56</v>
-      </c>
-      <c r="B53" s="6"/>
-      <c r="F53" s="12">
-        <v>3.8203E-5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>58</v>
       </c>
       <c r="B54" s="6"/>
       <c r="F54" s="12">
-        <v>1.1141E-14</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3.8203E-5</v>
+      </c>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B55" s="6"/>
       <c r="F55" s="12">
+        <v>1.1141E-14</v>
+      </c>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="F56" s="12">
         <v>-1.1141E-14</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B56" s="6"/>
-      <c r="F56" s="12"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="9" t="s">
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="6"/>
+      <c r="F57" s="12">
+        <v>3.3423999999999997E-14</v>
+      </c>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="6"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>18</v>
-      </c>
-      <c r="C59" s="6">
-        <v>-9.3643999999999997E-4</v>
-      </c>
-      <c r="D59" s="6">
-        <v>6.2724000000000005E-4</v>
-      </c>
-      <c r="E59" s="6">
-        <v>-7.9299000000000001E-5</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>33</v>
-      </c>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6">
-        <v>-9.3643999999999997E-4</v>
-      </c>
-      <c r="E60" s="6">
-        <v>-9.6071000000000004E-4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>34</v>
       </c>
       <c r="C61" s="6">
         <v>-9.3643999999999997E-4</v>
       </c>
+      <c r="D61" s="6">
+        <v>6.2724000000000005E-4</v>
+      </c>
       <c r="E61" s="6">
+        <v>-7.9299000000000001E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6">
+        <v>-9.3643999999999997E-4</v>
+      </c>
+      <c r="E62" s="6">
+        <v>-9.6071000000000004E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="6">
+        <v>-9.3643999999999997E-4</v>
+      </c>
+      <c r="E63" s="6">
         <v>1.5179000000000001E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="9" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="6">
+        <v>-1.7323999999999999E-4</v>
+      </c>
+      <c r="G64" s="6">
+        <v>4.8149999999999998E-5</v>
+      </c>
+      <c r="H64" s="6">
+        <v>-6.1882000000000001E-5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>66</v>
-      </c>
-      <c r="B65" s="6"/>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
-      <c r="F65" s="6">
-        <v>0.1191</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="6">
-        <v>-0.17849999999999999</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>67</v>
       </c>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
       <c r="F67" s="6">
-        <v>12.385999999999999</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.1191</v>
+      </c>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6">
-        <v>0.81820000000000004</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.17849999999999999</v>
+      </c>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6">
-        <v>0.2999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12.385999999999999</v>
+      </c>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
       <c r="E70" s="6"/>
       <c r="F70" s="6">
-        <v>0.3306</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.81820000000000004</v>
+      </c>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
-        <v>71</v>
+      <c r="F71" s="6">
+        <v>0.2999</v>
+      </c>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>70</v>
       </c>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
       <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>66</v>
-      </c>
+      <c r="F72" s="6">
+        <v>0.3306</v>
+      </c>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
       <c r="E73" s="6"/>
-      <c r="F73" s="6">
-        <v>0.68069999999999997</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>65</v>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
-      <c r="F74" s="6">
-        <v>-1.3599999999999999E-2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
       <c r="F75" s="6">
-        <v>90.748699999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.68069999999999997</v>
+      </c>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
       <c r="F76" s="6">
-        <v>3.2086000000000001</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.3599999999999999E-2</v>
+      </c>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
       <c r="F77" s="6">
-        <v>0.98870000000000002</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+        <v>90.748699999999999</v>
+      </c>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6">
-        <v>0.63880000000000003</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3.2086000000000001</v>
+      </c>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>69</v>
+      </c>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
-      <c r="F79" s="6"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="9" t="s">
-        <v>72</v>
+      <c r="F79" s="6">
+        <v>0.98870000000000002</v>
+      </c>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>70</v>
       </c>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>73</v>
-      </c>
+      <c r="F80" s="6">
+        <v>0.63880000000000003</v>
+      </c>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
-      <c r="F81" s="6">
-        <v>75.870999999999995</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>74</v>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
-      <c r="F82" s="6">
-        <v>1.4200000000000001E-2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>75</v>
-      </c>
-      <c r="B83" s="6">
-        <v>-4.4668999999999999E-13</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B83" s="6"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
       <c r="F83" s="6">
-        <v>276.39269999999999</v>
+        <v>75.870999999999995</v>
       </c>
       <c r="G83" s="6"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H83" s="6"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
       <c r="F84" s="6">
-        <v>3.2787999999999999</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>77</v>
-      </c>
-      <c r="B85" s="6"/>
+        <v>75</v>
+      </c>
+      <c r="B85" s="6">
+        <v>-4.4668999999999999E-13</v>
+      </c>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
       <c r="F85" s="6">
-        <v>276.52589999999998</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+        <v>276.39269999999999</v>
+      </c>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
       <c r="F86" s="6">
+        <v>3.2787999999999999</v>
+      </c>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>77</v>
+      </c>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6">
+        <v>276.52589999999998</v>
+      </c>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>78</v>
+      </c>
+      <c r="B88" s="6"/>
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6">
         <v>132.62020000000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>79</v>
       </c>
-      <c r="F87">
+      <c r="F89">
         <v>3.0599999999999999E-2</v>
       </c>
-      <c r="G87" t="s">
+      <c r="I89" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>80</v>
       </c>
-      <c r="F89" s="6">
+      <c r="F91" s="6">
         <v>-2.1473E-4</v>
       </c>
-      <c r="G89" t="s">
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>